<commit_message>
updated design documents for 5/20/23 milestone submission
</commit_message>
<xml_diff>
--- a/planning-docs/CST-451FunctionalRequirementStories.xlsx
+++ b/planning-docs/CST-451FunctionalRequirementStories.xlsx
@@ -11,12 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="68">
   <si>
     <t>Project Title: Little Offices - Capstone Project
 Author/PM: Daniel Cender
-Release #: 1
-Sprint #: 1</t>
+Release #: 0.4 5/20/23
+Sprint #: 4</t>
   </si>
   <si>
     <t>User Stories</t>
@@ -43,6 +43,9 @@
     <t>Assigned To</t>
   </si>
   <si>
+    <t>Delivery Status</t>
+  </si>
+  <si>
     <t>F1</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
   </si>
   <si>
     <t>Myself</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
   <si>
     <t>F2</t>
@@ -124,6 +130,9 @@
     <t>so I can visualize my placement on the map</t>
   </si>
   <si>
+    <t>Cut From Scope</t>
+  </si>
+  <si>
     <t>F8</t>
   </si>
   <si>
@@ -158,6 +167,9 @@
   </si>
   <si>
     <t>so that I can communicate verbally</t>
+  </si>
+  <si>
+    <t>Failed to Deliver on Time</t>
   </si>
   <si>
     <t>F11</t>
@@ -580,7 +592,8 @@
     <col customWidth="1" min="5" max="5" width="44.71"/>
     <col customWidth="1" min="6" max="6" width="13.14"/>
     <col customWidth="1" min="7" max="7" width="18.14"/>
-    <col customWidth="1" min="8" max="26" width="8.0"/>
+    <col customWidth="1" min="8" max="8" width="22.29"/>
+    <col customWidth="1" min="9" max="26" width="8.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -599,6 +612,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" ht="18.0" customHeight="1">
       <c r="A3" s="8" t="s">
@@ -622,336 +636,384 @@
       <c r="G3" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="H3" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="13">
         <v>2.0</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F5" s="13">
         <v>2.0</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6" s="13">
         <v>1.5</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="12" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F7" s="13">
         <v>1.5</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F8" s="13">
         <v>1.5</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F9" s="13">
         <v>1.5</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F10" s="13">
         <v>2.0</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F11" s="13">
         <v>3.0</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F12" s="13">
         <v>4.0</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F13" s="13">
         <v>4.0</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F14" s="13">
         <v>2.0</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F15" s="13">
         <v>2.0</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F16" s="13">
         <v>2.0</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B17" s="14"/>
       <c r="C17" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F17" s="13">
         <v>2.0</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F18" s="13">
         <v>2.0</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19">
@@ -965,6 +1027,7 @@
         <v>33</v>
       </c>
       <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
     </row>
     <row r="20">
       <c r="A20" s="14"/>

</xml_diff>